<commit_message>
add henan hebei 2/12 0-24
</commit_message>
<xml_diff>
--- a/NCP/data/unchecked/manual_collect/china/hebei/hebeiCaseStatistics_20200211.xlsx
+++ b/NCP/data/unchecked/manual_collect/china/hebei/hebeiCaseStatistics_20200211.xlsx
@@ -5,16 +5,19 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\yiqing\data\hebei\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\yiqing\pkuvis.github.io\NCP\data\unchecked\manual_collect\china\hebei\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F54C04-D1E4-4914-810E-8FFD891329E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752ECD69-879A-4689-96B2-A67C5CD22F75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$AN$183</definedName>
+  </definedNames>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -783,7 +786,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="yyyy/m/d\ h:mm;@"/>
+    <numFmt numFmtId="176" formatCode="yyyy/m/d\ h:mm;@"/>
   </numFmts>
   <fonts count="6">
     <font>
@@ -865,7 +868,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="22" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1158,10 +1161,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AN183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1487,7 +1491,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:40">
+    <row r="4" spans="1:40" hidden="1">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1552,7 +1556,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:40">
+    <row r="5" spans="1:40" hidden="1">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -1617,7 +1621,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:40">
+    <row r="6" spans="1:40" hidden="1">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1682,7 +1686,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:40">
+    <row r="7" spans="1:40" hidden="1">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -1747,7 +1751,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:40">
+    <row r="8" spans="1:40" hidden="1">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1812,7 +1816,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:40">
+    <row r="9" spans="1:40" hidden="1">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -1877,7 +1881,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:40">
+    <row r="10" spans="1:40" hidden="1">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1942,7 +1946,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="11" spans="1:40">
+    <row r="11" spans="1:40" hidden="1">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -2007,7 +2011,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:40">
+    <row r="12" spans="1:40" hidden="1">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2072,7 +2076,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="13" spans="1:40">
+    <row r="13" spans="1:40" hidden="1">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -2137,7 +2141,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:40">
+    <row r="14" spans="1:40" hidden="1">
       <c r="A14">
         <v>12</v>
       </c>
@@ -2202,7 +2206,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:40">
+    <row r="15" spans="1:40" hidden="1">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -2267,7 +2271,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:40">
+    <row r="16" spans="1:40" hidden="1">
       <c r="A16">
         <v>14</v>
       </c>
@@ -2332,7 +2336,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:33" hidden="1">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -2397,7 +2401,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:33" hidden="1">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2462,7 +2466,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:33" hidden="1">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -2527,7 +2531,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:33" hidden="1">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2592,7 +2596,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:33" hidden="1">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -2657,7 +2661,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:33" hidden="1">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2722,7 +2726,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:33" hidden="1">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -2787,7 +2791,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:33" hidden="1">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2852,7 +2856,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:33" hidden="1">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -2986,7 +2990,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:33" hidden="1">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -3051,7 +3055,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:33" hidden="1">
       <c r="A28">
         <v>26</v>
       </c>
@@ -3116,7 +3120,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:33" hidden="1">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -3181,7 +3185,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:33" hidden="1">
       <c r="A30">
         <v>28</v>
       </c>
@@ -3246,7 +3250,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:33" hidden="1">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -3311,7 +3315,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:33" hidden="1">
       <c r="A32">
         <v>30</v>
       </c>
@@ -3376,7 +3380,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:33" hidden="1">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -3441,7 +3445,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:33" hidden="1">
       <c r="A34">
         <v>32</v>
       </c>
@@ -3506,7 +3510,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:33" hidden="1">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -3571,7 +3575,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="36" spans="1:33">
+    <row r="36" spans="1:33" hidden="1">
       <c r="A36">
         <v>34</v>
       </c>
@@ -3636,7 +3640,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="37" spans="1:33">
+    <row r="37" spans="1:33" hidden="1">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -3701,7 +3705,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="38" spans="1:33">
+    <row r="38" spans="1:33" hidden="1">
       <c r="A38">
         <v>36</v>
       </c>
@@ -3766,7 +3770,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:33">
+    <row r="39" spans="1:33" hidden="1">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -3831,7 +3835,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="40" spans="1:33">
+    <row r="40" spans="1:33" hidden="1">
       <c r="A40">
         <v>38</v>
       </c>
@@ -3974,7 +3978,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="42" spans="1:33">
+    <row r="42" spans="1:33" hidden="1">
       <c r="A42">
         <v>40</v>
       </c>
@@ -4039,7 +4043,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="43" spans="1:33">
+    <row r="43" spans="1:33" hidden="1">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -4104,7 +4108,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:33">
+    <row r="44" spans="1:33" hidden="1">
       <c r="A44">
         <v>42</v>
       </c>
@@ -4169,7 +4173,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:33" hidden="1">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -4234,7 +4238,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:33" hidden="1">
       <c r="A46">
         <v>44</v>
       </c>
@@ -4299,7 +4303,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:33" hidden="1">
       <c r="A47" s="3">
         <v>45</v>
       </c>
@@ -4364,7 +4368,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="48" spans="1:33">
+    <row r="48" spans="1:33" hidden="1">
       <c r="A48">
         <v>46</v>
       </c>
@@ -4498,7 +4502,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:33" hidden="1">
       <c r="A50">
         <v>48</v>
       </c>
@@ -4563,7 +4567,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:33" hidden="1">
       <c r="A51" s="3">
         <v>49</v>
       </c>
@@ -4628,7 +4632,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:33" hidden="1">
       <c r="A52">
         <v>50</v>
       </c>
@@ -4693,7 +4697,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:33" hidden="1">
       <c r="A53" s="3">
         <v>51</v>
       </c>
@@ -4758,7 +4762,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:33" hidden="1">
       <c r="A54">
         <v>52</v>
       </c>
@@ -4823,7 +4827,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:33" hidden="1">
       <c r="A55" s="3">
         <v>53</v>
       </c>
@@ -4888,7 +4892,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:33" hidden="1">
       <c r="A56">
         <v>54</v>
       </c>
@@ -4953,7 +4957,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:33" hidden="1">
       <c r="A57" s="3">
         <v>55</v>
       </c>
@@ -5018,7 +5022,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:33" hidden="1">
       <c r="A58">
         <v>56</v>
       </c>
@@ -5083,7 +5087,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="59" spans="1:33">
+    <row r="59" spans="1:33" hidden="1">
       <c r="A59" s="3">
         <v>57</v>
       </c>
@@ -5148,7 +5152,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="60" spans="1:33">
+    <row r="60" spans="1:33" hidden="1">
       <c r="A60">
         <v>58</v>
       </c>
@@ -5213,7 +5217,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="61" spans="1:33">
+    <row r="61" spans="1:33" hidden="1">
       <c r="A61" s="3">
         <v>59</v>
       </c>
@@ -5278,7 +5282,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="62" spans="1:33">
+    <row r="62" spans="1:33" hidden="1">
       <c r="A62">
         <v>60</v>
       </c>
@@ -5343,7 +5347,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:33">
+    <row r="63" spans="1:33" hidden="1">
       <c r="A63" s="3">
         <v>61</v>
       </c>
@@ -5408,7 +5412,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="64" spans="1:33">
+    <row r="64" spans="1:33" hidden="1">
       <c r="A64">
         <v>62</v>
       </c>
@@ -5473,7 +5477,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="1:33">
+    <row r="65" spans="1:33" hidden="1">
       <c r="A65" s="3">
         <v>63</v>
       </c>
@@ -5538,7 +5542,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="66" spans="1:33">
+    <row r="66" spans="1:33" hidden="1">
       <c r="A66">
         <v>64</v>
       </c>
@@ -5603,7 +5607,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:33">
+    <row r="67" spans="1:33" hidden="1">
       <c r="A67" s="3">
         <v>65</v>
       </c>
@@ -5740,7 +5744,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="69" spans="1:33">
+    <row r="69" spans="1:33" hidden="1">
       <c r="A69" s="3">
         <v>67</v>
       </c>
@@ -5805,7 +5809,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:33">
+    <row r="70" spans="1:33" hidden="1">
       <c r="A70">
         <v>68</v>
       </c>
@@ -5870,7 +5874,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="71" spans="1:33">
+    <row r="71" spans="1:33" hidden="1">
       <c r="A71" s="3">
         <v>69</v>
       </c>
@@ -5935,7 +5939,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="72" spans="1:33">
+    <row r="72" spans="1:33" hidden="1">
       <c r="A72">
         <v>70</v>
       </c>
@@ -6000,7 +6004,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="73" spans="1:33">
+    <row r="73" spans="1:33" hidden="1">
       <c r="A73" s="3">
         <v>71</v>
       </c>
@@ -6065,7 +6069,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="74" spans="1:33">
+    <row r="74" spans="1:33" hidden="1">
       <c r="A74">
         <v>72</v>
       </c>
@@ -6130,7 +6134,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="75" spans="1:33">
+    <row r="75" spans="1:33" hidden="1">
       <c r="A75" s="3">
         <v>73</v>
       </c>
@@ -6195,7 +6199,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="1:33">
+    <row r="76" spans="1:33" hidden="1">
       <c r="A76">
         <v>74</v>
       </c>
@@ -6260,7 +6264,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="77" spans="1:33">
+    <row r="77" spans="1:33" hidden="1">
       <c r="A77" s="3">
         <v>75</v>
       </c>
@@ -6325,7 +6329,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="78" spans="1:33">
+    <row r="78" spans="1:33" hidden="1">
       <c r="A78">
         <v>76</v>
       </c>
@@ -6390,7 +6394,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="79" spans="1:33">
+    <row r="79" spans="1:33" hidden="1">
       <c r="A79" s="3">
         <v>77</v>
       </c>
@@ -6455,7 +6459,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="80" spans="1:33">
+    <row r="80" spans="1:33" hidden="1">
       <c r="A80">
         <v>78</v>
       </c>
@@ -6520,7 +6524,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="81" spans="1:33">
+    <row r="81" spans="1:33" hidden="1">
       <c r="A81" s="3">
         <v>79</v>
       </c>
@@ -6585,7 +6589,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="82" spans="1:33">
+    <row r="82" spans="1:33" hidden="1">
       <c r="A82">
         <v>80</v>
       </c>
@@ -6650,7 +6654,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="83" spans="1:33">
+    <row r="83" spans="1:33" hidden="1">
       <c r="A83" s="3">
         <v>81</v>
       </c>
@@ -6715,7 +6719,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="84" spans="1:33">
+    <row r="84" spans="1:33" hidden="1">
       <c r="A84">
         <v>82</v>
       </c>
@@ -6780,7 +6784,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="85" spans="1:33">
+    <row r="85" spans="1:33" hidden="1">
       <c r="A85" s="3">
         <v>83</v>
       </c>
@@ -6845,7 +6849,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="86" spans="1:33">
+    <row r="86" spans="1:33" hidden="1">
       <c r="A86">
         <v>84</v>
       </c>
@@ -6910,7 +6914,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="87" spans="1:33">
+    <row r="87" spans="1:33" hidden="1">
       <c r="A87" s="3">
         <v>85</v>
       </c>
@@ -7050,7 +7054,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="89" spans="1:33">
+    <row r="89" spans="1:33" hidden="1">
       <c r="A89" s="3">
         <v>87</v>
       </c>
@@ -7115,7 +7119,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="90" spans="1:33">
+    <row r="90" spans="1:33" hidden="1">
       <c r="A90">
         <v>88</v>
       </c>
@@ -7180,7 +7184,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="91" spans="1:33">
+    <row r="91" spans="1:33" hidden="1">
       <c r="A91" s="3">
         <v>89</v>
       </c>
@@ -7245,7 +7249,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="92" spans="1:33">
+    <row r="92" spans="1:33" hidden="1">
       <c r="A92">
         <v>90</v>
       </c>
@@ -7310,7 +7314,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="93" spans="1:33">
+    <row r="93" spans="1:33" hidden="1">
       <c r="A93" s="3">
         <v>91</v>
       </c>
@@ -7375,7 +7379,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="94" spans="1:33">
+    <row r="94" spans="1:33" hidden="1">
       <c r="A94">
         <v>92</v>
       </c>
@@ -7440,7 +7444,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="95" spans="1:33">
+    <row r="95" spans="1:33" hidden="1">
       <c r="A95" s="3">
         <v>93</v>
       </c>
@@ -7505,7 +7509,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="96" spans="1:33">
+    <row r="96" spans="1:33" hidden="1">
       <c r="A96">
         <v>94</v>
       </c>
@@ -7570,7 +7574,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="97" spans="1:33">
+    <row r="97" spans="1:33" hidden="1">
       <c r="A97" s="3">
         <v>95</v>
       </c>
@@ -7635,7 +7639,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="98" spans="1:33">
+    <row r="98" spans="1:33" hidden="1">
       <c r="A98">
         <v>96</v>
       </c>
@@ -7700,7 +7704,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="99" spans="1:33">
+    <row r="99" spans="1:33" hidden="1">
       <c r="A99" s="3">
         <v>97</v>
       </c>
@@ -7765,7 +7769,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="100" spans="1:33">
+    <row r="100" spans="1:33" hidden="1">
       <c r="A100">
         <v>98</v>
       </c>
@@ -7830,7 +7834,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="101" spans="1:33">
+    <row r="101" spans="1:33" hidden="1">
       <c r="A101" s="3">
         <v>99</v>
       </c>
@@ -7895,7 +7899,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="102" spans="1:33">
+    <row r="102" spans="1:33" hidden="1">
       <c r="A102">
         <v>100</v>
       </c>
@@ -7960,7 +7964,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="103" spans="1:33">
+    <row r="103" spans="1:33" hidden="1">
       <c r="A103" s="3">
         <v>101</v>
       </c>
@@ -8025,7 +8029,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="104" spans="1:33">
+    <row r="104" spans="1:33" hidden="1">
       <c r="A104">
         <v>102</v>
       </c>
@@ -8090,7 +8094,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="105" spans="1:33">
+    <row r="105" spans="1:33" hidden="1">
       <c r="A105" s="3">
         <v>103</v>
       </c>
@@ -8155,7 +8159,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="106" spans="1:33">
+    <row r="106" spans="1:33" hidden="1">
       <c r="A106">
         <v>104</v>
       </c>
@@ -8220,7 +8224,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="107" spans="1:33">
+    <row r="107" spans="1:33" hidden="1">
       <c r="A107" s="3">
         <v>105</v>
       </c>
@@ -8285,7 +8289,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="108" spans="1:33">
+    <row r="108" spans="1:33" hidden="1">
       <c r="A108">
         <v>106</v>
       </c>
@@ -8350,7 +8354,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="109" spans="1:33">
+    <row r="109" spans="1:33" hidden="1">
       <c r="A109" s="3">
         <v>107</v>
       </c>
@@ -8415,7 +8419,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="110" spans="1:33">
+    <row r="110" spans="1:33" hidden="1">
       <c r="A110">
         <v>108</v>
       </c>
@@ -8483,7 +8487,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="111" spans="1:33">
+    <row r="111" spans="1:33" hidden="1">
       <c r="A111" s="3">
         <v>109</v>
       </c>
@@ -8548,7 +8552,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="112" spans="1:33">
+    <row r="112" spans="1:33" hidden="1">
       <c r="A112">
         <v>110</v>
       </c>
@@ -8688,7 +8692,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="114" spans="1:33">
+    <row r="114" spans="1:33" hidden="1">
       <c r="A114">
         <v>112</v>
       </c>
@@ -8753,7 +8757,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="115" spans="1:33">
+    <row r="115" spans="1:33" hidden="1">
       <c r="A115" s="3">
         <v>113</v>
       </c>
@@ -8818,7 +8822,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="116" spans="1:33">
+    <row r="116" spans="1:33" hidden="1">
       <c r="A116">
         <v>114</v>
       </c>
@@ -8883,7 +8887,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="117" spans="1:33">
+    <row r="117" spans="1:33" hidden="1">
       <c r="A117" s="3">
         <v>115</v>
       </c>
@@ -8948,7 +8952,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="118" spans="1:33">
+    <row r="118" spans="1:33" hidden="1">
       <c r="A118">
         <v>116</v>
       </c>
@@ -9013,7 +9017,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="119" spans="1:33">
+    <row r="119" spans="1:33" hidden="1">
       <c r="A119" s="3">
         <v>117</v>
       </c>
@@ -9078,7 +9082,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="120" spans="1:33">
+    <row r="120" spans="1:33" hidden="1">
       <c r="A120">
         <v>118</v>
       </c>
@@ -9143,7 +9147,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="121" spans="1:33">
+    <row r="121" spans="1:33" hidden="1">
       <c r="A121" s="3">
         <v>119</v>
       </c>
@@ -9208,7 +9212,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="122" spans="1:33">
+    <row r="122" spans="1:33" hidden="1">
       <c r="A122">
         <v>120</v>
       </c>
@@ -9273,7 +9277,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="123" spans="1:33">
+    <row r="123" spans="1:33" hidden="1">
       <c r="A123" s="3">
         <v>121</v>
       </c>
@@ -9338,7 +9342,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="124" spans="1:33">
+    <row r="124" spans="1:33" hidden="1">
       <c r="A124">
         <v>122</v>
       </c>
@@ -9403,7 +9407,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="125" spans="1:33">
+    <row r="125" spans="1:33" hidden="1">
       <c r="A125" s="3">
         <v>123</v>
       </c>
@@ -9468,7 +9472,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="126" spans="1:33">
+    <row r="126" spans="1:33" hidden="1">
       <c r="A126">
         <v>124</v>
       </c>
@@ -9533,7 +9537,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="127" spans="1:33">
+    <row r="127" spans="1:33" hidden="1">
       <c r="A127" s="3">
         <v>125</v>
       </c>
@@ -9598,7 +9602,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="128" spans="1:33">
+    <row r="128" spans="1:33" hidden="1">
       <c r="A128">
         <v>126</v>
       </c>
@@ -9663,7 +9667,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="129" spans="1:33">
+    <row r="129" spans="1:33" hidden="1">
       <c r="A129" s="3">
         <v>127</v>
       </c>
@@ -9800,7 +9804,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="131" spans="1:33">
+    <row r="131" spans="1:33" hidden="1">
       <c r="A131" s="3">
         <v>129</v>
       </c>
@@ -9865,7 +9869,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="132" spans="1:33">
+    <row r="132" spans="1:33" hidden="1">
       <c r="A132">
         <v>130</v>
       </c>
@@ -9930,7 +9934,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="133" spans="1:33">
+    <row r="133" spans="1:33" hidden="1">
       <c r="A133" s="3">
         <v>131</v>
       </c>
@@ -9995,7 +9999,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="134" spans="1:33">
+    <row r="134" spans="1:33" hidden="1">
       <c r="A134">
         <v>132</v>
       </c>
@@ -10060,7 +10064,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="135" spans="1:33">
+    <row r="135" spans="1:33" hidden="1">
       <c r="A135" s="3">
         <v>133</v>
       </c>
@@ -10125,7 +10129,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="136" spans="1:33">
+    <row r="136" spans="1:33" hidden="1">
       <c r="A136">
         <v>134</v>
       </c>
@@ -10190,7 +10194,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="137" spans="1:33">
+    <row r="137" spans="1:33" hidden="1">
       <c r="A137" s="3">
         <v>135</v>
       </c>
@@ -10255,7 +10259,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="138" spans="1:33">
+    <row r="138" spans="1:33" hidden="1">
       <c r="A138">
         <v>136</v>
       </c>
@@ -10320,7 +10324,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="139" spans="1:33">
+    <row r="139" spans="1:33" hidden="1">
       <c r="A139" s="3">
         <v>137</v>
       </c>
@@ -10385,7 +10389,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="140" spans="1:33">
+    <row r="140" spans="1:33" hidden="1">
       <c r="A140">
         <v>138</v>
       </c>
@@ -10450,7 +10454,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="141" spans="1:33">
+    <row r="141" spans="1:33" hidden="1">
       <c r="A141" s="3">
         <v>139</v>
       </c>
@@ -10584,7 +10588,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="143" spans="1:33">
+    <row r="143" spans="1:33" hidden="1">
       <c r="A143" s="3">
         <v>141</v>
       </c>
@@ -10649,7 +10653,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="144" spans="1:33">
+    <row r="144" spans="1:33" hidden="1">
       <c r="A144">
         <v>142</v>
       </c>
@@ -10714,7 +10718,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="145" spans="1:33">
+    <row r="145" spans="1:33" hidden="1">
       <c r="A145" s="3">
         <v>143</v>
       </c>
@@ -10779,7 +10783,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="146" spans="1:33">
+    <row r="146" spans="1:33" hidden="1">
       <c r="A146">
         <v>144</v>
       </c>
@@ -10844,7 +10848,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="147" spans="1:33">
+    <row r="147" spans="1:33" hidden="1">
       <c r="A147" s="3">
         <v>145</v>
       </c>
@@ -10909,7 +10913,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="148" spans="1:33">
+    <row r="148" spans="1:33" hidden="1">
       <c r="A148">
         <v>146</v>
       </c>
@@ -10974,7 +10978,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="149" spans="1:33">
+    <row r="149" spans="1:33" hidden="1">
       <c r="A149" s="3">
         <v>147</v>
       </c>
@@ -11039,7 +11043,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="150" spans="1:33">
+    <row r="150" spans="1:33" hidden="1">
       <c r="A150">
         <v>148</v>
       </c>
@@ -11104,7 +11108,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="151" spans="1:33">
+    <row r="151" spans="1:33" hidden="1">
       <c r="A151" s="3">
         <v>149</v>
       </c>
@@ -11169,7 +11173,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="152" spans="1:33">
+    <row r="152" spans="1:33" hidden="1">
       <c r="A152">
         <v>150</v>
       </c>
@@ -11234,7 +11238,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="153" spans="1:33">
+    <row r="153" spans="1:33" hidden="1">
       <c r="A153" s="3">
         <v>151</v>
       </c>
@@ -11299,7 +11303,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="154" spans="1:33">
+    <row r="154" spans="1:33" hidden="1">
       <c r="A154">
         <v>152</v>
       </c>
@@ -11364,7 +11368,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="155" spans="1:33">
+    <row r="155" spans="1:33" hidden="1">
       <c r="A155" s="3">
         <v>153</v>
       </c>
@@ -11429,7 +11433,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="156" spans="1:33">
+    <row r="156" spans="1:33" hidden="1">
       <c r="A156">
         <v>154</v>
       </c>
@@ -11494,7 +11498,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="157" spans="1:33">
+    <row r="157" spans="1:33" hidden="1">
       <c r="A157" s="3">
         <v>155</v>
       </c>
@@ -11559,7 +11563,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="158" spans="1:33">
+    <row r="158" spans="1:33" hidden="1">
       <c r="A158">
         <v>156</v>
       </c>
@@ -11705,7 +11709,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="160" spans="1:33">
+    <row r="160" spans="1:33" hidden="1">
       <c r="A160">
         <v>158</v>
       </c>
@@ -11770,7 +11774,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="161" spans="1:33">
+    <row r="161" spans="1:33" hidden="1">
       <c r="A161" s="3">
         <v>159</v>
       </c>
@@ -11835,7 +11839,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="162" spans="1:33">
+    <row r="162" spans="1:33" hidden="1">
       <c r="A162">
         <v>160</v>
       </c>
@@ -11900,7 +11904,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="163" spans="1:33">
+    <row r="163" spans="1:33" hidden="1">
       <c r="A163" s="3">
         <v>161</v>
       </c>
@@ -11965,7 +11969,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="164" spans="1:33">
+    <row r="164" spans="1:33" hidden="1">
       <c r="A164">
         <v>162</v>
       </c>
@@ -12030,7 +12034,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="165" spans="1:33">
+    <row r="165" spans="1:33" hidden="1">
       <c r="A165" s="3">
         <v>163</v>
       </c>
@@ -12095,7 +12099,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="166" spans="1:33">
+    <row r="166" spans="1:33" hidden="1">
       <c r="A166">
         <v>164</v>
       </c>
@@ -12160,7 +12164,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="167" spans="1:33">
+    <row r="167" spans="1:33" hidden="1">
       <c r="A167" s="3">
         <v>165</v>
       </c>
@@ -12225,7 +12229,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="168" spans="1:33">
+    <row r="168" spans="1:33" hidden="1">
       <c r="A168">
         <v>166</v>
       </c>
@@ -12290,7 +12294,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="169" spans="1:33">
+    <row r="169" spans="1:33" hidden="1">
       <c r="A169" s="3">
         <v>167</v>
       </c>
@@ -12430,7 +12434,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="171" spans="1:33">
+    <row r="171" spans="1:33" hidden="1">
       <c r="A171" s="3">
         <v>169</v>
       </c>
@@ -12495,7 +12499,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="172" spans="1:33">
+    <row r="172" spans="1:33" hidden="1">
       <c r="A172">
         <v>170</v>
       </c>
@@ -12560,7 +12564,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="173" spans="1:33">
+    <row r="173" spans="1:33" hidden="1">
       <c r="A173" s="3">
         <v>171</v>
       </c>
@@ -12625,7 +12629,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="174" spans="1:33">
+    <row r="174" spans="1:33" hidden="1">
       <c r="A174">
         <v>172</v>
       </c>
@@ -12690,7 +12694,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="175" spans="1:33">
+    <row r="175" spans="1:33" hidden="1">
       <c r="A175" s="3">
         <v>173</v>
       </c>
@@ -12755,7 +12759,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="176" spans="1:33">
+    <row r="176" spans="1:33" hidden="1">
       <c r="A176">
         <v>174</v>
       </c>
@@ -12820,7 +12824,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="177" spans="1:33">
+    <row r="177" spans="1:33" hidden="1">
       <c r="A177" s="3">
         <v>175</v>
       </c>
@@ -12885,7 +12889,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="178" spans="1:33">
+    <row r="178" spans="1:33" hidden="1">
       <c r="A178">
         <v>176</v>
       </c>
@@ -12950,7 +12954,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="179" spans="1:33">
+    <row r="179" spans="1:33" hidden="1">
       <c r="A179" s="3">
         <v>177</v>
       </c>
@@ -13015,7 +13019,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="180" spans="1:33">
+    <row r="180" spans="1:33" hidden="1">
       <c r="A180">
         <v>178</v>
       </c>
@@ -13080,7 +13084,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="181" spans="1:33">
+    <row r="181" spans="1:33" hidden="1">
       <c r="A181" s="3">
         <v>179</v>
       </c>
@@ -13281,6 +13285,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A2:AN183" xr:uid="{C5DA3823-D22A-4E58-AE0D-CAA9A2B219E0}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="城市级"/>
+        <filter val="省级"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="V3" r:id="rId1" xr:uid="{ED947FDD-F5C0-4E62-BBE9-65B055AF884D}"/>
@@ -13466,5 +13478,6 @@
     <hyperlink ref="V182" r:id="rId181" xr:uid="{0AE991B4-DFF8-41BB-A8A4-71F33F19369D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId182"/>
 </worksheet>
 </file>
</xml_diff>